<commit_message>
Actualizada información de infraestructuras de Atlántico
</commit_message>
<xml_diff>
--- a/Infraestructura/MatrizInfraestructurasNuevas_2019.xlsx
+++ b/Infraestructura/MatrizInfraestructurasNuevas_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea Ospina Patiño\Documents\GitHub\Dotaciones2019\Infraestructura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118E5C2B-D0C0-438A-9B50-936311521DCC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D4C3CD-7845-45DA-9F65-C3670D374829}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28785" windowHeight="16515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="396">
   <si>
     <t xml:space="preserve">Regional </t>
   </si>
@@ -1398,6 +1398,12 @@
   </si>
   <si>
     <t>El Fondo de Adaptacion reporta que la dotacion la entrega la Gobernación de Bolívar, verificar con la regional</t>
+  </si>
+  <si>
+    <t>Solicitada a Capital social</t>
+  </si>
+  <si>
+    <t>Existe una carta de compromiso de la Gobernación</t>
   </si>
 </sst>
 </file>
@@ -1867,6 +1873,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1899,9 +1908,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2190,12 +2196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <pane ySplit="2" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2223,13 +2228,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="32" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="56" t="s">
         <v>359</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
       <c r="L1" s="33"/>
       <c r="N1" s="33"/>
       <c r="Q1" s="48"/>
@@ -2286,7 +2291,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="39" customFormat="1" ht="149.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="39" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36">
         <v>1</v>
       </c>
@@ -2339,7 +2344,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="39" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="39" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <v>2</v>
       </c>
@@ -2392,7 +2397,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36">
         <v>3</v>
       </c>
@@ -2441,7 +2446,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="39" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="39" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
         <v>4</v>
       </c>
@@ -2494,7 +2499,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="39" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="36">
         <v>5</v>
       </c>
@@ -2545,7 +2550,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="39" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="39" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="36">
         <v>6</v>
       </c>
@@ -2594,7 +2599,7 @@
       <c r="Q8" s="47"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="1:18" s="39" customFormat="1" ht="54.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="39" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
         <v>7</v>
       </c>
@@ -2647,7 +2652,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="39" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="39" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="36">
         <v>8</v>
       </c>
@@ -2700,7 +2705,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="39" customFormat="1" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="39" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <v>9</v>
       </c>
@@ -2753,7 +2758,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="39" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
         <v>10</v>
       </c>
@@ -2802,7 +2807,7 @@
       <c r="Q12" s="47"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="36">
         <v>11</v>
       </c>
@@ -2851,7 +2856,7 @@
       <c r="Q13" s="47"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="36">
         <v>12</v>
       </c>
@@ -2905,7 +2910,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="36">
         <v>13</v>
       </c>
@@ -2958,7 +2963,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="39" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="39" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>14</v>
       </c>
@@ -3011,7 +3016,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
         <v>15</v>
       </c>
@@ -3060,7 +3065,7 @@
       <c r="Q17" s="47"/>
       <c r="R17" s="16"/>
     </row>
-    <row r="18" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="36">
         <v>16</v>
       </c>
@@ -3109,7 +3114,7 @@
       <c r="Q18" s="47"/>
       <c r="R18" s="16"/>
     </row>
-    <row r="19" spans="1:18" s="39" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="36">
         <v>17</v>
       </c>
@@ -3158,7 +3163,7 @@
       <c r="Q19" s="47"/>
       <c r="R19" s="16"/>
     </row>
-    <row r="20" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="36">
         <v>18</v>
       </c>
@@ -3207,7 +3212,7 @@
       <c r="Q20" s="47"/>
       <c r="R20" s="16"/>
     </row>
-    <row r="21" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>19</v>
       </c>
@@ -3256,7 +3261,7 @@
       <c r="Q21" s="47"/>
       <c r="R21" s="16"/>
     </row>
-    <row r="22" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <v>20</v>
       </c>
@@ -3305,7 +3310,7 @@
       <c r="Q22" s="47"/>
       <c r="R22" s="16"/>
     </row>
-    <row r="23" spans="1:18" s="39" customFormat="1" ht="118.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" s="39" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36">
         <v>21</v>
       </c>
@@ -3358,7 +3363,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36">
         <v>22</v>
       </c>
@@ -3869,7 +3874,7 @@
       <c r="Q34" s="49"/>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="36">
         <v>33</v>
       </c>
@@ -3918,7 +3923,7 @@
       <c r="Q35" s="49"/>
       <c r="R35" s="16"/>
     </row>
-    <row r="36" spans="1:18" s="39" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="36">
         <v>34</v>
       </c>
@@ -3966,7 +3971,7 @@
       <c r="Q36" s="49"/>
       <c r="R36" s="16"/>
     </row>
-    <row r="37" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="36">
         <v>35</v>
       </c>
@@ -4014,7 +4019,7 @@
       <c r="Q37" s="49"/>
       <c r="R37" s="16"/>
     </row>
-    <row r="38" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="36">
         <v>36</v>
       </c>
@@ -4062,7 +4067,7 @@
       <c r="Q38" s="49"/>
       <c r="R38" s="16"/>
     </row>
-    <row r="39" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="36">
         <v>37</v>
       </c>
@@ -4110,7 +4115,7 @@
       <c r="Q39" s="49"/>
       <c r="R39" s="16"/>
     </row>
-    <row r="40" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="36">
         <v>38</v>
       </c>
@@ -4159,7 +4164,7 @@
       <c r="Q40" s="49"/>
       <c r="R40" s="16"/>
     </row>
-    <row r="41" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="36">
         <v>39</v>
       </c>
@@ -4207,7 +4212,7 @@
       <c r="Q41" s="49"/>
       <c r="R41" s="16"/>
     </row>
-    <row r="42" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="36">
         <v>40</v>
       </c>
@@ -4255,7 +4260,7 @@
       <c r="Q42" s="49"/>
       <c r="R42" s="16"/>
     </row>
-    <row r="43" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="36">
         <v>41</v>
       </c>
@@ -4304,7 +4309,7 @@
       <c r="Q43" s="49"/>
       <c r="R43" s="16"/>
     </row>
-    <row r="44" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="36">
         <v>42</v>
       </c>
@@ -4352,7 +4357,7 @@
       <c r="Q44" s="49"/>
       <c r="R44" s="16"/>
     </row>
-    <row r="45" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="36">
         <v>43</v>
       </c>
@@ -4401,7 +4406,7 @@
       <c r="Q45" s="49"/>
       <c r="R45" s="16"/>
     </row>
-    <row r="46" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="36">
         <v>44</v>
       </c>
@@ -4449,7 +4454,7 @@
       <c r="Q46" s="49"/>
       <c r="R46" s="16"/>
     </row>
-    <row r="47" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="36">
         <v>45</v>
       </c>
@@ -4497,7 +4502,7 @@
       <c r="Q47" s="49"/>
       <c r="R47" s="16"/>
     </row>
-    <row r="48" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="36">
         <v>46</v>
       </c>
@@ -4545,7 +4550,7 @@
       <c r="Q48" s="49"/>
       <c r="R48" s="16"/>
     </row>
-    <row r="49" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="36">
         <v>47</v>
       </c>
@@ -4587,7 +4592,7 @@
       <c r="Q49" s="49"/>
       <c r="R49" s="16"/>
     </row>
-    <row r="50" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="36">
         <v>48</v>
       </c>
@@ -4636,7 +4641,7 @@
       <c r="Q50" s="49"/>
       <c r="R50" s="16"/>
     </row>
-    <row r="51" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="36">
         <v>49</v>
       </c>
@@ -4684,7 +4689,7 @@
       <c r="Q51" s="49"/>
       <c r="R51" s="16"/>
     </row>
-    <row r="52" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="36">
         <v>50</v>
       </c>
@@ -4732,7 +4737,7 @@
       <c r="Q52" s="49"/>
       <c r="R52" s="16"/>
     </row>
-    <row r="53" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="36">
         <v>51</v>
       </c>
@@ -4780,7 +4785,7 @@
       <c r="Q53" s="49"/>
       <c r="R53" s="16"/>
     </row>
-    <row r="54" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="36">
         <v>52</v>
       </c>
@@ -4828,7 +4833,7 @@
       <c r="Q54" s="49"/>
       <c r="R54" s="16"/>
     </row>
-    <row r="55" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="36">
         <v>53</v>
       </c>
@@ -4876,7 +4881,7 @@
       <c r="Q55" s="49"/>
       <c r="R55" s="16"/>
     </row>
-    <row r="56" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="36">
         <v>54</v>
       </c>
@@ -4924,7 +4929,7 @@
       <c r="Q56" s="49"/>
       <c r="R56" s="16"/>
     </row>
-    <row r="57" spans="1:18" s="39" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" s="39" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="36">
         <v>55</v>
       </c>
@@ -4975,7 +4980,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="58" spans="1:18" s="39" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" s="39" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="36">
         <v>56</v>
       </c>
@@ -5025,7 +5030,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="59" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="36">
         <v>57</v>
       </c>
@@ -5077,7 +5082,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="60" spans="1:18" s="39" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" s="39" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="36">
         <v>58</v>
       </c>
@@ -5127,7 +5132,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="39" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="36">
         <v>59</v>
       </c>
@@ -5180,7 +5185,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="62" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="36">
         <v>60</v>
       </c>
@@ -5234,7 +5239,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="36">
         <v>61</v>
       </c>
@@ -5283,7 +5288,7 @@
       <c r="Q63" s="49"/>
       <c r="R63" s="16"/>
     </row>
-    <row r="64" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="36">
         <v>62</v>
       </c>
@@ -5331,7 +5336,7 @@
       <c r="Q64" s="49"/>
       <c r="R64" s="16"/>
     </row>
-    <row r="65" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="36">
         <v>64</v>
       </c>
@@ -5378,7 +5383,7 @@
       <c r="Q65" s="49"/>
       <c r="R65" s="16"/>
     </row>
-    <row r="66" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="36">
         <v>65</v>
       </c>
@@ -5424,7 +5429,7 @@
       <c r="Q66" s="49"/>
       <c r="R66" s="16"/>
     </row>
-    <row r="67" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="36">
         <v>66</v>
       </c>
@@ -5473,7 +5478,7 @@
       <c r="Q67" s="49"/>
       <c r="R67" s="16"/>
     </row>
-    <row r="68" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="36">
         <v>67</v>
       </c>
@@ -5519,7 +5524,7 @@
       <c r="Q68" s="49"/>
       <c r="R68" s="16"/>
     </row>
-    <row r="69" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="36">
         <v>68</v>
       </c>
@@ -5565,7 +5570,7 @@
       <c r="Q69" s="49"/>
       <c r="R69" s="16"/>
     </row>
-    <row r="70" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="36">
         <v>69</v>
       </c>
@@ -5662,8 +5667,12 @@
       </c>
       <c r="O71" s="16"/>
       <c r="P71" s="45"/>
-      <c r="Q71" s="49"/>
-      <c r="R71" s="16"/>
+      <c r="Q71" s="51" t="s">
+        <v>378</v>
+      </c>
+      <c r="R71" s="16" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="72" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="36">
@@ -5711,8 +5720,12 @@
       </c>
       <c r="O72" s="16"/>
       <c r="P72" s="45"/>
-      <c r="Q72" s="49"/>
-      <c r="R72" s="16"/>
+      <c r="Q72" s="51" t="s">
+        <v>378</v>
+      </c>
+      <c r="R72" s="16" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="73" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="36">
@@ -5760,8 +5773,12 @@
       </c>
       <c r="O73" s="16"/>
       <c r="P73" s="45"/>
-      <c r="Q73" s="49"/>
-      <c r="R73" s="16"/>
+      <c r="Q73" s="51" t="s">
+        <v>378</v>
+      </c>
+      <c r="R73" s="16" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="74" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="36">
@@ -5809,10 +5826,14 @@
       </c>
       <c r="O74" s="16"/>
       <c r="P74" s="45"/>
-      <c r="Q74" s="49"/>
-      <c r="R74" s="16"/>
-    </row>
-    <row r="75" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Q74" s="51" t="s">
+        <v>378</v>
+      </c>
+      <c r="R74" s="16" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A75" s="36">
         <v>74</v>
       </c>
@@ -5863,7 +5884,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="76" spans="1:18" s="39" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A76" s="36">
         <v>75</v>
       </c>
@@ -5914,7 +5935,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="77" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="36">
         <v>76</v>
       </c>
@@ -5963,7 +5984,7 @@
       <c r="Q77" s="49"/>
       <c r="R77" s="16"/>
     </row>
-    <row r="78" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="36">
         <v>77</v>
       </c>
@@ -6012,7 +6033,7 @@
       <c r="Q78" s="49"/>
       <c r="R78" s="16"/>
     </row>
-    <row r="79" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="36">
         <v>78</v>
       </c>
@@ -6061,7 +6082,7 @@
       <c r="Q79" s="49"/>
       <c r="R79" s="16"/>
     </row>
-    <row r="80" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="36">
         <v>79</v>
       </c>
@@ -6110,7 +6131,7 @@
       <c r="Q80" s="49"/>
       <c r="R80" s="16"/>
     </row>
-    <row r="81" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="36">
         <v>80</v>
       </c>
@@ -6159,7 +6180,7 @@
       <c r="Q81" s="49"/>
       <c r="R81" s="16"/>
     </row>
-    <row r="82" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="36">
         <v>81</v>
       </c>
@@ -6209,7 +6230,7 @@
       <c r="Q82" s="49"/>
       <c r="R82" s="16"/>
     </row>
-    <row r="83" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="36">
         <v>82</v>
       </c>
@@ -6258,7 +6279,7 @@
       <c r="Q83" s="49"/>
       <c r="R83" s="16"/>
     </row>
-    <row r="84" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="36">
         <v>83</v>
       </c>
@@ -6307,7 +6328,7 @@
       <c r="Q84" s="49"/>
       <c r="R84" s="16"/>
     </row>
-    <row r="85" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="36">
         <v>84</v>
       </c>
@@ -6356,7 +6377,7 @@
       <c r="Q85" s="49"/>
       <c r="R85" s="16"/>
     </row>
-    <row r="86" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="36">
         <v>85</v>
       </c>
@@ -6405,7 +6426,7 @@
       <c r="Q86" s="49"/>
       <c r="R86" s="16"/>
     </row>
-    <row r="87" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="36">
         <v>86</v>
       </c>
@@ -6454,7 +6475,7 @@
       <c r="Q87" s="49"/>
       <c r="R87" s="16"/>
     </row>
-    <row r="88" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="36">
         <v>87</v>
       </c>
@@ -6503,7 +6524,7 @@
       <c r="Q88" s="49"/>
       <c r="R88" s="16"/>
     </row>
-    <row r="89" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="36">
         <v>88</v>
       </c>
@@ -6552,7 +6573,7 @@
       <c r="Q89" s="49"/>
       <c r="R89" s="16"/>
     </row>
-    <row r="90" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="36">
         <v>89</v>
       </c>
@@ -6601,7 +6622,7 @@
       <c r="Q90" s="49"/>
       <c r="R90" s="16"/>
     </row>
-    <row r="91" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="36">
         <v>90</v>
       </c>
@@ -6650,7 +6671,7 @@
       <c r="Q91" s="49"/>
       <c r="R91" s="16"/>
     </row>
-    <row r="92" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="36">
         <v>91</v>
       </c>
@@ -6699,7 +6720,7 @@
       <c r="Q92" s="49"/>
       <c r="R92" s="16"/>
     </row>
-    <row r="93" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="36">
         <v>92</v>
       </c>
@@ -6740,7 +6761,7 @@
       <c r="Q93" s="49"/>
       <c r="R93" s="16"/>
     </row>
-    <row r="94" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="36">
         <v>93</v>
       </c>
@@ -6781,7 +6802,7 @@
       <c r="Q94" s="49"/>
       <c r="R94" s="16"/>
     </row>
-    <row r="95" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="36">
         <v>94</v>
       </c>
@@ -6822,7 +6843,7 @@
       <c r="Q95" s="49"/>
       <c r="R95" s="16"/>
     </row>
-    <row r="96" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="36">
         <v>95</v>
       </c>
@@ -6863,7 +6884,7 @@
       <c r="Q96" s="49"/>
       <c r="R96" s="16"/>
     </row>
-    <row r="97" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="36">
         <v>96</v>
       </c>
@@ -6904,7 +6925,7 @@
       <c r="Q97" s="49"/>
       <c r="R97" s="16"/>
     </row>
-    <row r="98" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="36">
         <v>97</v>
       </c>
@@ -6945,7 +6966,7 @@
       <c r="Q98" s="49"/>
       <c r="R98" s="16"/>
     </row>
-    <row r="99" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="36">
         <v>98</v>
       </c>
@@ -6986,7 +7007,7 @@
       <c r="Q99" s="49"/>
       <c r="R99" s="16"/>
     </row>
-    <row r="100" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="36">
         <v>99</v>
       </c>
@@ -7027,7 +7048,7 @@
       <c r="Q100" s="49"/>
       <c r="R100" s="16"/>
     </row>
-    <row r="101" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="36">
         <v>100</v>
       </c>
@@ -7078,7 +7099,7 @@
       <c r="Q101" s="49"/>
       <c r="R101" s="16"/>
     </row>
-    <row r="102" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="36">
         <v>101</v>
       </c>
@@ -7127,7 +7148,7 @@
       <c r="Q102" s="49"/>
       <c r="R102" s="16"/>
     </row>
-    <row r="103" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="36">
         <v>102</v>
       </c>
@@ -7176,7 +7197,7 @@
       <c r="Q103" s="49"/>
       <c r="R103" s="16"/>
     </row>
-    <row r="104" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="36">
         <v>103</v>
       </c>
@@ -7225,7 +7246,7 @@
       <c r="Q104" s="49"/>
       <c r="R104" s="16"/>
     </row>
-    <row r="105" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="36">
         <v>104</v>
       </c>
@@ -7274,7 +7295,7 @@
       <c r="Q105" s="49"/>
       <c r="R105" s="16"/>
     </row>
-    <row r="106" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="36">
         <v>105</v>
       </c>
@@ -7324,7 +7345,7 @@
       <c r="Q106" s="49"/>
       <c r="R106" s="16"/>
     </row>
-    <row r="107" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="36">
         <v>106</v>
       </c>
@@ -7373,7 +7394,7 @@
       <c r="Q107" s="49"/>
       <c r="R107" s="16"/>
     </row>
-    <row r="108" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="36">
         <v>107</v>
       </c>
@@ -7422,7 +7443,7 @@
       <c r="Q108" s="49"/>
       <c r="R108" s="16"/>
     </row>
-    <row r="109" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="36">
         <v>108</v>
       </c>
@@ -7471,7 +7492,7 @@
       <c r="Q109" s="49"/>
       <c r="R109" s="16"/>
     </row>
-    <row r="110" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="36">
         <v>109</v>
       </c>
@@ -7520,7 +7541,7 @@
       <c r="Q110" s="49"/>
       <c r="R110" s="16"/>
     </row>
-    <row r="111" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="36">
         <v>110</v>
       </c>
@@ -7569,7 +7590,7 @@
       <c r="Q111" s="49"/>
       <c r="R111" s="16"/>
     </row>
-    <row r="112" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="36">
         <v>111</v>
       </c>
@@ -7618,7 +7639,7 @@
       <c r="Q112" s="49"/>
       <c r="R112" s="16"/>
     </row>
-    <row r="113" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="36">
         <v>112</v>
       </c>
@@ -7669,7 +7690,7 @@
       <c r="Q113" s="49"/>
       <c r="R113" s="16"/>
     </row>
-    <row r="114" spans="1:18" s="39" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="36">
         <v>113</v>
       </c>
@@ -7721,7 +7742,7 @@
       <c r="Q114" s="49"/>
       <c r="R114" s="16"/>
     </row>
-    <row r="115" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="36">
         <v>114</v>
       </c>
@@ -7770,7 +7791,7 @@
       <c r="Q115" s="49"/>
       <c r="R115" s="16"/>
     </row>
-    <row r="116" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="36">
         <v>115</v>
       </c>
@@ -7814,7 +7835,7 @@
       <c r="Q116" s="49"/>
       <c r="R116" s="16"/>
     </row>
-    <row r="117" spans="1:18" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="36">
         <v>116</v>
       </c>
@@ -7858,7 +7879,7 @@
       <c r="Q117" s="49"/>
       <c r="R117" s="16"/>
     </row>
-    <row r="118" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="36">
         <v>117</v>
       </c>
@@ -7902,7 +7923,7 @@
       <c r="Q118" s="49"/>
       <c r="R118" s="16"/>
     </row>
-    <row r="119" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="36">
         <v>118</v>
       </c>
@@ -7946,7 +7967,7 @@
       <c r="Q119" s="49"/>
       <c r="R119" s="16"/>
     </row>
-    <row r="120" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="36">
         <v>119</v>
       </c>
@@ -7990,7 +8011,7 @@
       <c r="Q120" s="49"/>
       <c r="R120" s="16"/>
     </row>
-    <row r="121" spans="1:18" s="39" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="36">
         <v>120</v>
       </c>
@@ -8034,7 +8055,7 @@
       <c r="Q121" s="49"/>
       <c r="R121" s="16"/>
     </row>
-    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" s="55" t="s">
         <v>241</v>
       </c>
@@ -8055,7 +8076,7 @@
       <c r="P122" s="55"/>
       <c r="Q122" s="40"/>
     </row>
-    <row r="123" spans="1:18" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="55" t="s">
         <v>240</v>
       </c>
@@ -8128,14 +8149,6 @@
       <c r="A141" s="42"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:S123" xr:uid="{86055434-BEF0-4C37-8FD0-1DD243E3A7C1}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Atlántico"/>
-        <filter val="Atlántico "/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="A123:P123"/>
     <mergeCell ref="A122:P122"/>
@@ -8541,15 +8554,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
     </row>
     <row r="7" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -9003,15 +9016,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -9037,15 +9050,15 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -9117,15 +9130,15 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="59" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -9358,15 +9371,15 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="59" t="s">
         <v>280</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -9461,15 +9474,15 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="59" t="s">
         <v>281</v>
       </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
     </row>
     <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -9668,18 +9681,18 @@
       <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="63" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="62"/>
+      <c r="E7" s="63"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="64" t="s">
         <v>283</v>
       </c>
-      <c r="E8" s="63"/>
+      <c r="E8" s="64"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -9716,10 +9729,10 @@
       <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="65" t="s">
         <v>286</v>
       </c>
-      <c r="E11" s="64"/>
+      <c r="E11" s="65"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" s="11" t="s">
@@ -9758,16 +9771,16 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="66" t="s">
         <v>270</v>
       </c>
-      <c r="E17" s="65"/>
+      <c r="E17" s="66"/>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="67" t="s">
         <v>283</v>
       </c>
-      <c r="E18" s="66"/>
+      <c r="E18" s="67"/>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" s="12" t="s">
@@ -9786,10 +9799,10 @@
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="E21" s="61"/>
+      <c r="E21" s="62"/>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" s="13" t="s">

</xml_diff>